<commit_message>
Hele hoop zooi met neerwaartse onderdelen
</commit_message>
<xml_diff>
--- a/Main/Voorbeeldschip_Deelopdracht_8_V3.xlsx
+++ b/Main/Voorbeeldschip_Deelopdracht_8_V3.xlsx
@@ -1254,7 +1254,7 @@
         </is>
       </c>
       <c r="D16" s="10" t="n">
-        <v>3.915667654722501</v>
+        <v>3.927530225934194</v>
       </c>
     </row>
     <row r="17" ht="35.4" customHeight="1">
@@ -1534,7 +1534,7 @@
         </is>
       </c>
       <c r="D37" s="26" t="n">
-        <v>70.88124375022056</v>
+        <v>70.8812805182052</v>
       </c>
     </row>
     <row r="38" ht="18" customHeight="1">
@@ -1549,7 +1549,7 @@
         </is>
       </c>
       <c r="D38" s="26" t="n">
-        <v>5.935282149104807e-06</v>
+        <v>0.000107979679917548</v>
       </c>
     </row>
     <row r="39">
@@ -1564,7 +1564,7 @@
         </is>
       </c>
       <c r="D39" s="26" t="n">
-        <v>6.29751709268565</v>
+        <v>6.285594842359499</v>
       </c>
     </row>
     <row r="41">
@@ -1685,7 +1685,7 @@
         </is>
       </c>
       <c r="D50" s="14" t="n">
-        <v>-926077.0562391379</v>
+        <v>-934935.5889284521</v>
       </c>
     </row>
     <row r="51">
@@ -1700,7 +1700,7 @@
         </is>
       </c>
       <c r="D51" s="14" t="n">
-        <v>-1429.991103786975</v>
+        <v>-26015.60933293588</v>
       </c>
     </row>
     <row r="52" ht="40.95" customHeight="1">
@@ -1791,7 +1791,7 @@
         </is>
       </c>
       <c r="D58" s="10" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" ht="14.4" customHeight="1">

</xml_diff>